<commit_message>
update: add new column (6 quantity units and rate production) on table
</commit_message>
<xml_diff>
--- a/src/assets/files/template-upload-gentani.xlsx
+++ b/src/assets/files/template-upload-gentani.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC30736D-5E74-40E8-9C0B-1749FE9A9B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7A591A-CC63-47B6-9302-689879747549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>material_no</t>
   </si>
   <si>
-    <t>quantity</t>
+    <t>quantity_fortuner</t>
+  </si>
+  <si>
+    <t>quantity_zenix</t>
+  </si>
+  <si>
+    <t>quantity_innova</t>
   </si>
   <si>
     <t>plant</t>
@@ -35,7 +41,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0."/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -45,6 +56,11 @@
     <font>
       <sz val="11.5"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -67,9 +83,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -406,31 +437,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="1.25" right="1.25" top="1" bottom="0.79166666666666696" header="0.25" footer="0.25"/>
 </worksheet>
 </file>
</xml_diff>